<commit_message>
Created robot drive code
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>DIO</t>
   </si>
@@ -38,12 +38,27 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Left Joystick</t>
+  </si>
+  <si>
+    <t>Right Joystick</t>
+  </si>
+  <si>
+    <t>Left  Drive</t>
+  </si>
+  <si>
+    <t>Right Drive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,73 +454,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B41"/>
+  <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -513,14 +543,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added encoders to robot code.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>DIO</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>Right Drive</t>
+  </si>
+  <si>
+    <t>left a</t>
+  </si>
+  <si>
+    <t>right b</t>
+  </si>
+  <si>
+    <t>right a</t>
+  </si>
+  <si>
+    <t>left b</t>
   </si>
 </sst>
 </file>
@@ -457,7 +469,7 @@
   <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +489,9 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
       <c r="D3">
         <v>0</v>
       </c>
@@ -488,6 +503,9 @@
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
       <c r="D4">
         <v>1</v>
       </c>
@@ -499,10 +517,16 @@
       <c r="A5">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added in all the hardware references to the robot code. Began work on the dashboard. Updated the robot pinout.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Robot" sheetId="1" r:id="rId1"/>
+    <sheet name="Driver Station" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>DIO</t>
   </si>
@@ -55,16 +56,112 @@
     <t>Right Drive</t>
   </si>
   <si>
-    <t>left a</t>
-  </si>
-  <si>
-    <t>right b</t>
-  </si>
-  <si>
-    <t>right a</t>
-  </si>
-  <si>
-    <t>left b</t>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Fire Ready</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Autonomous Selector</t>
+  </si>
+  <si>
+    <t>Arm Pos - Shoot</t>
+  </si>
+  <si>
+    <t>Arm Pos - Manual Up</t>
+  </si>
+  <si>
+    <t>Arm Pos - Manual Down</t>
+  </si>
+  <si>
+    <t>Arm Pos - Cross Defense</t>
+  </si>
+  <si>
+    <t>Arm Pos - Low Bar</t>
+  </si>
+  <si>
+    <t>Arm Pos - Human Player Load</t>
+  </si>
+  <si>
+    <t>Intake - In</t>
+  </si>
+  <si>
+    <t>Intake - Out</t>
+  </si>
+  <si>
+    <t>Lift - Retract</t>
+  </si>
+  <si>
+    <t>Lift - Extend</t>
+  </si>
+  <si>
+    <t>Drive Encoder - Right A</t>
+  </si>
+  <si>
+    <t>Drive Encoder - Right B</t>
+  </si>
+  <si>
+    <t>Drive Encoder - Left A</t>
+  </si>
+  <si>
+    <t>Drive Encoder - Left B</t>
+  </si>
+  <si>
+    <t>Intake Motor</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Pressure Sensor</t>
+  </si>
+  <si>
+    <t>Lift Motor w/ Magnetic Encoder</t>
+  </si>
+  <si>
+    <t>Arm Motor w/ Potentiometer</t>
+  </si>
+  <si>
+    <t>IMU - Analog Devices ADIS1448</t>
+  </si>
+  <si>
+    <t>Lift Extend Motor</t>
+  </si>
+  <si>
+    <t>PCM</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Yes - Wire to 20A Breaker</t>
+  </si>
+  <si>
+    <t>Shooter - Extend</t>
+  </si>
+  <si>
+    <t>Shooter - Retract</t>
+  </si>
+  <si>
+    <t>Arm Lock</t>
+  </si>
+  <si>
+    <t>Arm Unlock</t>
+  </si>
+  <si>
+    <t>Ethernet</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 2 - Model B - Vision Processing</t>
   </si>
 </sst>
 </file>
@@ -100,8 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,16 +223,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>151175</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>46400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -156,8 +256,68 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5838824" y="151175"/>
+          <a:off x="11391899" y="1379900"/>
           <a:ext cx="6753225" cy="6649675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4781550" y="219075"/>
+          <a:ext cx="5486400" cy="5486400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,15 +626,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E41"/>
+  <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="201" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -484,13 +648,26 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -498,13 +675,28 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -512,118 +704,193 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -631,27 +898,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -663,6 +930,9 @@
       <c r="A33">
         <v>0</v>
       </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -679,24 +949,340 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="240" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit of progress. Working on drive base control in Periodic Tasks.vi
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>DIO</t>
   </si>
@@ -32,9 +32,6 @@
     <t>CAN</t>
   </si>
   <si>
-    <t>I2C</t>
-  </si>
-  <si>
     <t>RS-232</t>
   </si>
   <si>
@@ -162,12 +159,15 @@
   </si>
   <si>
     <t>Raspberry Pi 2 - Model B - Vision Processing</t>
+  </si>
+  <si>
+    <t>XDP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,10 +197,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -223,16 +226,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>46400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>952499</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -256,7 +259,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11391899" y="1379900"/>
+          <a:off x="5295899" y="1141775"/>
           <a:ext cx="6753225" cy="6649675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -628,14 +631,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView zoomScale="201" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -643,23 +654,20 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -667,28 +675,25 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -696,22 +701,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -719,13 +724,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -733,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -771,13 +776,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -785,13 +790,13 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -799,13 +804,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,13 +818,13 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,13 +832,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,10 +878,10 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,10 +889,10 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -895,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -923,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="240" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="240" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
@@ -973,7 +978,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -984,13 +989,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1009,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1020,7 +1025,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1031,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1042,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1053,7 +1058,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1133,7 +1138,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -1144,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1155,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1166,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1177,7 +1182,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1188,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1199,7 +1204,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1210,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1221,7 +1226,7 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -1232,7 +1237,7 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -1243,7 +1248,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29">
         <v>9</v>
@@ -1254,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>10</v>

</xml_diff>

<commit_message>
Added special button controls for driver to change direction. Added controls for operator. Added arm control operated through the operator.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>DIO</t>
   </si>
@@ -162,12 +162,15 @@
   </si>
   <si>
     <t>XDP</t>
+  </si>
+  <si>
+    <t>Lock disengaged</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,10 +203,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +662,10 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="2"/>
       <c r="K2" t="s">
         <v>5</v>
       </c>
@@ -689,7 +692,7 @@
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M3" t="s">
@@ -744,6 +747,9 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -967,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="240" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="240" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished arm control code.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>DIO</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Lock disengaged</t>
+  </si>
+  <si>
+    <t>Arm Position</t>
   </si>
 </sst>
 </file>
@@ -634,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,6 +951,9 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Shooter working. Arm mode setting finished. Removed Network Variables from Control Board update loop.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>DIO</t>
   </si>
@@ -68,21 +68,6 @@
     <t>Autonomous Selector</t>
   </si>
   <si>
-    <t>Arm Pos - Shoot</t>
-  </si>
-  <si>
-    <t>Arm Pos - Manual Up</t>
-  </si>
-  <si>
-    <t>Arm Pos - Manual Down</t>
-  </si>
-  <si>
-    <t>Arm Pos - Cross Defense</t>
-  </si>
-  <si>
-    <t>Arm Pos - Low Bar</t>
-  </si>
-  <si>
     <t>Arm Pos - Human Player Load</t>
   </si>
   <si>
@@ -168,6 +153,24 @@
   </si>
   <si>
     <t>Arm Position</t>
+  </si>
+  <si>
+    <t>Arm Pos - Shoot Batter</t>
+  </si>
+  <si>
+    <t>Arm Pos - Shooter Close</t>
+  </si>
+  <si>
+    <t>Arm Pos - Shoot Far</t>
+  </si>
+  <si>
+    <t>Arm Pos - Manual</t>
+  </si>
+  <si>
+    <t>Arm Pos - Low Bar / Goal</t>
+  </si>
+  <si>
+    <t>Manual Arm Position</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -673,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -681,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -690,16 +693,16 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="M3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -707,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -719,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -730,13 +733,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -744,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -752,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -788,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -805,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -819,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,13 +830,13 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -841,13 +844,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,10 +890,10 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,10 +901,10 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -953,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="240" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1018,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1037,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1048,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1059,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1070,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1172,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1183,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1194,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1205,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1216,7 +1222,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1227,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1238,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -1249,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -1260,7 +1266,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D29">
         <v>9</v>
@@ -1271,7 +1277,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D30">
         <v>10</v>

</xml_diff>

<commit_message>
Calibrated arm sensor and fixed various bugs.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>DIO</t>
   </si>
@@ -113,9 +113,6 @@
     <t>IMU - Analog Devices ADIS1448</t>
   </si>
   <si>
-    <t>Lift Extend Motor</t>
-  </si>
-  <si>
     <t>PCM</t>
   </si>
   <si>
@@ -128,18 +125,6 @@
     <t>Yes - Wire to 20A Breaker</t>
   </si>
   <si>
-    <t>Shooter - Extend</t>
-  </si>
-  <si>
-    <t>Shooter - Retract</t>
-  </si>
-  <si>
-    <t>Arm Lock</t>
-  </si>
-  <si>
-    <t>Arm Unlock</t>
-  </si>
-  <si>
     <t>Ethernet</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
     <t>XDP</t>
   </si>
   <si>
-    <t>Lock disengaged</t>
-  </si>
-  <si>
     <t>Arm Position</t>
   </si>
   <si>
@@ -171,6 +153,27 @@
   </si>
   <si>
     <t>Manual Arm Position</t>
+  </si>
+  <si>
+    <t>Shooter - Extend/Retract</t>
+  </si>
+  <si>
+    <t>Arm Latch - Lock/Unlock</t>
+  </si>
+  <si>
+    <t>Claw - Open</t>
+  </si>
+  <si>
+    <t>Claw - Close</t>
+  </si>
+  <si>
+    <t>Lock Engaged</t>
+  </si>
+  <si>
+    <t>Control Board</t>
+  </si>
+  <si>
+    <t>Matbotix Distance Sensor</t>
   </si>
 </sst>
 </file>
@@ -638,16 +641,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.85546875" bestFit="1" customWidth="1"/>
@@ -676,7 +682,7 @@
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -699,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -735,6 +741,12 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
@@ -755,13 +767,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -791,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
@@ -808,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -822,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -836,21 +851,18 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +905,7 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,10 +913,10 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,15 +986,19 @@
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -1018,13 +1034,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1043,7 +1059,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1065,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1076,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1178,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1189,7 +1205,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1200,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1222,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1233,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1310,6 +1326,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="55" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added drive base slew rate control. Added exception functionality for arm-autolock. Changed lock detection to unlock detection to prevent the arm from binding up. Fixed a bug with the arm momentarily locking when coming out of disable mode. Fixed a bug where half-speed operation would work only in normal arcade mode and not normal or split-axis arcade mode.
</commit_message>
<xml_diff>
--- a/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
+++ b/2016/2016 Robot/Electrical/2016 RoboRIO Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>DIO</t>
   </si>
@@ -234,12 +234,15 @@
   </si>
   <si>
     <t>Lift Extend Motor</t>
+  </si>
+  <si>
+    <t>Disable Slew Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,12 +286,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,7 +721,7 @@
   </sheetPr>
   <dimension ref="A2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -746,10 +749,10 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="4"/>
       <c r="K2" t="s">
         <v>5</v>
       </c>
@@ -799,7 +802,7 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="J4" t="s">
@@ -813,7 +816,7 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E5" t="s">
@@ -930,7 +933,7 @@
       <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D18">
@@ -1129,8 +1132,8 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1437,9 @@
       <c r="A31">
         <v>11</v>
       </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">

</xml_diff>